<commit_message>
kinetics stuff for difuego
</commit_message>
<xml_diff>
--- a/Experiments/221220_serine_titrate/output.xlsx
+++ b/Experiments/221220_serine_titrate/output.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryancardiff/Documents/Carothers/ARPA-E/Experiments/221220_serine_titrate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryancardiff/Documents/GitHub/WHISPR/Experiments/221220_serine_titrate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95F7DE6C-C864-2243-B11D-29C00BECCC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C457CE-44DD-5F4B-B014-6C3A31E617AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1100" windowWidth="27640" windowHeight="16340" xr2:uid="{B7E67C64-D74D-204A-861E-6D7F53143D6F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ser_1000</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Pyr_Rep3</t>
+  </si>
+  <si>
+    <t>Dilution</t>
   </si>
 </sst>
 </file>
@@ -179,9 +182,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -219,7 +222,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -325,7 +328,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -467,7 +470,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -475,15 +478,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E45EC61B-23EC-A443-9B2C-94C166603EF1}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:J6"/>
+    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>7</v>
       </c>
@@ -491,28 +494,31 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -523,28 +529,31 @@
         <v>24</v>
       </c>
       <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2">
         <v>8</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>286382.26</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1399359.52</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1038276.11</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>13587.35</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>23073.58</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>77764.87</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -555,28 +564,31 @@
         <v>24</v>
       </c>
       <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="E3">
         <v>8</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>426661.94</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>1187914.05</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1325894.92</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>13238.69</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>37128.239999999998</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>95930.44</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -587,28 +599,31 @@
         <v>24</v>
       </c>
       <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="E4">
         <v>8</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>227690.26</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>878193.63</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1304156.74</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>15813.28</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>28198.21</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>94330.74</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -619,28 +634,31 @@
         <v>24</v>
       </c>
       <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="E5">
         <v>8</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>425913.84</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>696886.41</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1227934.52</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>15630.32</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>11963.81</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>109659.4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -651,22 +669,25 @@
         <v>24</v>
       </c>
       <c r="D6">
+        <v>200</v>
+      </c>
+      <c r="E6">
         <v>8</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>282811.89</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>556227.85</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>11912.68</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>113488.7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -677,21 +698,24 @@
         <v>24</v>
       </c>
       <c r="D7">
+        <v>200</v>
+      </c>
+      <c r="E7">
         <v>8</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>629984.11</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>558911.91</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>145251.78</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>290358.34000000003</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>147902.65</v>
       </c>
     </row>

</xml_diff>